<commit_message>
Extendreport e cenarios de cadastro concluido.
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/testData/MassaDeDados.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/testData/MassaDeDados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.correia\git\projeto-tdd\src\main\java\br\com\rsinet\hub_tdd\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.correia\git\projeto-appium-tdd\src\main\java\br\com\rsinet\hub_tdd\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F861F0EB-8197-4DE8-A64A-79FB4BEAEDDA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCBFEC4-7F83-4DE9-A90D-0DEB6362BA1A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
   </bookViews>
@@ -219,7 +219,7 @@
     <t>HP Z3600 WIRELESS MOUSE</t>
   </si>
   <si>
-    <t>lucascarval90</t>
+    <t>lucascarvalh05</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Cenarios de busca por lupa sucesso e falha e busca por home sucesso criados.
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/testData/MassaDeDados.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/testData/MassaDeDados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.correia\git\projeto-appium-tdd\src\main\java\br\com\rsinet\hub_tdd\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2ACFA91-D408-455E-879A-1294A7B28114}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832A1729-F3D1-436C-B24D-3D5ECAEA7858}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
   <si>
     <t>lucascarvalho</t>
   </si>
@@ -69,18 +69,12 @@
     <t>1</t>
   </si>
   <si>
-    <t>HP</t>
-  </si>
-  <si>
     <t>fones</t>
   </si>
   <si>
     <t>Pesquisa efetuada com sucesso!</t>
   </si>
   <si>
-    <t>Compra efetuada com sucesso!</t>
-  </si>
-  <si>
     <t>Cadastro efetuado com sucesso!</t>
   </si>
   <si>
@@ -99,9 +93,6 @@
     <t>HP Chromebook 14 G1(ES)</t>
   </si>
   <si>
-    <t>Thank you for buying with Advantage</t>
-  </si>
-  <si>
     <t>UserName</t>
   </si>
   <si>
@@ -216,10 +207,13 @@
     <t>HP Z3600 Wireless Mouse</t>
   </si>
   <si>
-    <t>HP Z3600 WIRELESS MOUSE</t>
-  </si>
-  <si>
-    <t>lucascarvalh07</t>
+    <t>HP H2310 IN-EAR HEADSET</t>
+  </si>
+  <si>
+    <t>lucascarvalh23</t>
+  </si>
+  <si>
+    <t>HP ROAR MINI WIRELESS SPEAKER</t>
   </si>
 </sst>
 </file>
@@ -640,7 +634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B732072B-4DFA-4889-A7A4-3C1058C30EFF}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -662,35 +656,35 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="1"/>
       <c r="E1" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>1</v>
@@ -698,15 +692,15 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -714,15 +708,15 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
@@ -734,7 +728,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
@@ -746,7 +740,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -758,7 +752,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
@@ -770,7 +764,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
@@ -782,7 +776,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>6</v>
@@ -794,7 +788,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
@@ -806,7 +800,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>8</v>
@@ -818,7 +812,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
@@ -830,7 +824,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>10</v>
@@ -857,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B33322F-19DE-45EB-B55A-70A3D3B1968A}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,43 +866,43 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="1"/>
       <c r="D1" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -916,31 +910,31 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="1"/>
       <c r="D5" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -955,7 +949,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="1"/>
@@ -964,7 +958,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>12</v>
@@ -990,7 +984,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,43 +998,43 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="1"/>
       <c r="D1" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1050,7 +1044,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="1"/>
@@ -1059,10 +1053,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1092,13 +1086,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1106,7 +1100,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>

</xml_diff>